<commit_message>
Pegando o preço de um produto
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Python Impressionador\Projeto_PrecosAmazon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A80E3-7ED9-4EE6-B66F-2E231D2FE6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C33AD0C8-7A04-48F0-8FD4-D9E2559CEECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,35 +59,35 @@
     <t>Local</t>
   </si>
   <si>
-    <t>iPhone 11 Apple 64GB Preto</t>
+    <t>iPhone 15 Apple 128GB Preto</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.br/gp/aw/d/B0CP6CVJSG/?_encoding=UTF8&amp;pd_rd_plhdr=t&amp;aaxitk=71870feb0a4de624959d0dc6cd3143de&amp;hsa_cr_id=2734213800601&amp;qid=1751583756&amp;sr=1-2-9e67e56a-6f64-441f-a281-df67fc737124&amp;ref_=sbx_be_s_sparkle_dlcd_asin_1_img&amp;pd_rd_w=2UCbV&amp;content-id=amzn1.sym.da990715-51de-4373-b8ab-d245f18f3edf%3Aamzn1.sym.da990715-51de-4373-b8ab-d245f18f3edf&amp;pf_rd_p=da990715-51de-4373-b8ab-d245f18f3edf&amp;pf_rd_r=D3D8M9T0W18MAZZJM6Z8&amp;pd_rd_wg=EvWpu&amp;pd_rd_r=49a8f4fa-0d1f-47d6-afe7-8a6c94744c0c&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.americanas.com.br/apple-iphone-15-de-128gb-preto-174n0p87924z7261/p?idsku=7763713&amp;utm_source=YSMESP&amp;utm_medium=buscappc&amp;utm_campaign=celulares_3p&amp;utm_content=bp_pl_sh_go_aloc_digital_celulares_topitens_3p_aon25-00014&amp;utm_term=pla_shoppingpadrao&amp;gad_source=1&amp;gad_campaignid=22388929149&amp;gbraid=0AAAAAD37VppWcVmTKgnAlwmq47CtWjCxO&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2Ssnjp0NqiipnAJnKBFoSQZiWSwxJ4lUhNNkWkhXS1dUGeHBf25pXf8aAhrvEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.magazineluiza.com.br/apple-iphone-15-128gb-preto-61-48mp-ios-5g/p/238035600/te/ip15/?&amp;seller_id=magazineluiza&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_term=79684&amp;utm_campaign=google_eco_per_ven_pla_mob_apo_1p_te-csp&amp;utm_content=&amp;partner_id=79684&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22578732921&amp;gbraid=0AAAAAD4zZmTvhM3LLUO76XwjDkjAbe4ca&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SsbLJ7_-kwUaY-DHsgDCKDYJ50rBTUn43KmU8TLEQ8Hvp-T-P-oSAgaAn98EALw_wcB</t>
   </si>
   <si>
     <t>Smart TV LED 50'' LG Ultra HD 4K Thinq AI</t>
   </si>
   <si>
-    <t>https://www.amazon.com.br/IPHONE-11-PRETO-TELA-C%C3%82MERA/dp/B086VQTMPR/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+11&amp;qid=1606856566&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com.br/Smart-LG-Intelig%C3%AAncia-Artificial-Virtual/dp/B0877QDB3V/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=televis%C3%A3o&amp;qid=1606856629&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/1611315933?pfm_carac=iphone-11-64gb-preto-ios-4g-camera-12mp-apple&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/495161500?pfm_carac=smart-tv-led-pro-50-ultra-hd-4k-lg&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.magazineluiza.com.br/iphone-11-apple-64gb-preto-61-12mp-ios/p/155610500/te/ip11/</t>
-  </si>
-  <si>
-    <t>https://www.magazineluiza.com.br/smart-tv-uhd-4k-led-50-lg-50un7310psc-wi-fi-bluetooth-inteligencia-artificial-3-hdmi-2-usb/p/225376700/et/elit/?origin=autocomplete&amp;p=Smart%20TV%20LED%20PRO%2050%20Ultra%20HD%204K%20LG&amp;ranking=1&amp;typeclick=3&amp;ac_pos=header</t>
+    <t>https://www.amazon.com.br/LG-50NANO80T-Processador-Chromecast-integrado/dp/B0D3JB8GYZ/ref=asc_df_B0D3JB8GYZ?mcid=769db38cdb513c40a442f4c7cc227410&amp;tag=googleshopp00-20&amp;linkCode=df0&amp;hvadid=709964502896&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17184299404204777997&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1031811&amp;hvtargid=pla-2323939420537&amp;psc=1&amp;language=pt_BR&amp;gad_source=1</t>
+  </si>
+  <si>
+    <t>https://www.americanas.com.br/smart-tv-4k-50-polegadas-lg-uhd-50ut8050-processador-a5-ger7-ai-alexa-chromecast-integrado-otimizador-de-jogos-webos-24-controle-smart-magic-7507042514/p?idsku=5725301&amp;utm_source=YSMESP&amp;utm_medium=buscappc&amp;utm_campaign=alwayson-25&amp;utm_content=bp_pl_sh_go_aloc_digital_apostassortimento_3p_aon25-00234&amp;utm_term=pla_shopping&amp;gad_source=1&amp;gad_campaignid=22744334395&amp;gbraid=0AAAAAD37Vpp_JV01DVyUO7oovGs82Yucz&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SunsoJy03aCCv1IHpsRxNNoRQqvqLxcybiTTcbs3YwbiicYJS3uZWsaAmpdEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.magazineluiza.com.br/smart-tv-50-4k-lg-ultra-hd-50ut8050-com-processador-a5-ger7-ai-alexa-chromecast-integrado-otimizador-de-jogos-webos-24-e-controle-smart-magic/p/238617500/et/tves/?&amp;seller_id=magazineluiza&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_term=79710&amp;utm_campaign=google_eco_per_ven_pla_tc_apo_1p_et-csp&amp;utm_content=&amp;partner_id=79710&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22561248932&amp;gbraid=0AAAAAD4zZmTItqqzq1KWwBaXEdlBOIQCI&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SvijLU9hiNk_RLA5c6s1AMxr70tz3SwbtfO8u5P_6qLd55AzURost4aAiJtEALw_wcB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +109,7 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,10 +146,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -142,7 +156,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -159,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,26 +248,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,26 +283,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,11 +461,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,32 +490,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>5297</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -544,12 +526,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.com.br/gp/aw/d/B0CP6CVJSG/?_encoding=UTF8&amp;pd_rd_plhdr=t&amp;aaxitk=71870feb0a4de624959d0dc6cd3143de&amp;hsa_cr_id=2734213800601&amp;qid=1751583756&amp;sr=1-2-9e67e56a-6f64-441f-a281-df67fc737124&amp;ref_=sbx_be_s_sparkle_dlcd_asin_1_img&amp;pd_rd_w=2UCbV&amp;content-id=amzn1.sym.da990715-51de-4373-b8ab-d245f18f3edf%3Aamzn1.sym.da990715-51de-4373-b8ab-d245f18f3edf&amp;pf_rd_p=da990715-51de-4373-b8ab-d245f18f3edf&amp;pf_rd_r=D3D8M9T0W18MAZZJM6Z8&amp;pd_rd_wg=EvWpu&amp;pd_rd_r=49a8f4fa-0d1f-47d6-afe7-8a6c94744c0c&amp;th=1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://www.americanas.com.br/apple-iphone-15-de-128gb-preto-174n0p87924z7261/p?idsku=7763713&amp;utm_source=YSMESP&amp;utm_medium=buscappc&amp;utm_campaign=celulares_3p&amp;utm_content=bp_pl_sh_go_aloc_digital_celulares_topitens_3p_aon25-00014&amp;utm_term=pla_shoppingpadrao&amp;gad_source=1&amp;gad_campaignid=22388929149&amp;gbraid=0AAAAAD37VppWcVmTKgnAlwmq47CtWjCxO&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2Ssnjp0NqiipnAJnKBFoSQZiWSwxJ4lUhNNkWkhXS1dUGeHBf25pXf8aAhrvEALw_wcB" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://www.magazineluiza.com.br/apple-iphone-15-128gb-preto-61-48mp-ios-5g/p/238035600/te/ip15/?&amp;seller_id=magazineluiza&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_term=79684&amp;utm_campaign=google_eco_per_ven_pla_mob_apo_1p_te-csp&amp;utm_content=&amp;partner_id=79684&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22578732921&amp;gbraid=0AAAAAD4zZmTvhM3LLUO76XwjDkjAbe4ca&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SsbLJ7_-kwUaY-DHsgDCKDYJ50rBTUn43KmU8TLEQ8Hvp-T-P-oSAgaAn98EALw_wcB" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://www.amazon.com.br/LG-50NANO80T-Processador-Chromecast-integrado/dp/B0D3JB8GYZ/ref=asc_df_B0D3JB8GYZ?mcid=769db38cdb513c40a442f4c7cc227410&amp;tag=googleshopp00-20&amp;linkCode=df0&amp;hvadid=709964502896&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17184299404204777997&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1031811&amp;hvtargid=pla-2323939420537&amp;psc=1&amp;language=pt_BR&amp;gad_source=1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" display="https://www.americanas.com.br/smart-tv-4k-50-polegadas-lg-uhd-50ut8050-processador-a5-ger7-ai-alexa-chromecast-integrado-otimizador-de-jogos-webos-24-controle-smart-magic-7507042514/p?idsku=5725301&amp;utm_source=YSMESP&amp;utm_medium=buscappc&amp;utm_campaign=alwayson-25&amp;utm_content=bp_pl_sh_go_aloc_digital_apostassortimento_3p_aon25-00234&amp;utm_term=pla_shopping&amp;gad_source=1&amp;gad_campaignid=22744334395&amp;gbraid=0AAAAAD37Vpp_JV01DVyUO7oovGs82Yucz&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SunsoJy03aCCv1IHpsRxNNoRQqvqLxcybiTTcbs3YwbiicYJS3uZWsaAmpdEALw_wcB" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" display="https://www.magazineluiza.com.br/smart-tv-50-4k-lg-ultra-hd-50ut8050-com-processador-a5-ger7-ai-alexa-chromecast-integrado-otimizador-de-jogos-webos-24-e-controle-smart-magic/p/238617500/et/tves/?&amp;seller_id=magazineluiza&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_term=79710&amp;utm_campaign=google_eco_per_ven_pla_tc_apo_1p_et-csp&amp;utm_content=&amp;partner_id=79710&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22561248932&amp;gbraid=0AAAAAD4zZmTItqqzq1KWwBaXEdlBOIQCI&amp;gclid=Cj0KCQjw1JjDBhDjARIsABlM2SvijLU9hiNk_RLA5c6s1AMxr70tz3SwbtfO8u5P_6qLd55AzURost4aAiJtEALw_wcB" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>